<commit_message>
feat: make first comment..
</commit_message>
<xml_diff>
--- a/Sheets/LocalizationSheet.xlsx
+++ b/Sheets/LocalizationSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t xml:space="preserve">Выход</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prologue/firstComment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you dream of this ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приснится же такое…</t>
   </si>
 </sst>
 </file>
@@ -329,13 +338,14 @@
   <dimension ref="A2:H29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="3" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -441,11 +451,19 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
+    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
       <c r="G8" s="10"/>

</xml_diff>